<commit_message>
checking in working copy 10th version
</commit_message>
<xml_diff>
--- a/AgenticAI/story_teller_deepseek/qa.xlsx
+++ b/AgenticAI/story_teller_deepseek/qa.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Query</t>
   </si>
@@ -22,78 +22,85 @@
     <t>Answer</t>
   </si>
   <si>
-    <t>what is that one important reason one can participate this clinical trial?</t>
-  </si>
-  <si>
-    <t>what is the goal of the study?</t>
-  </si>
-  <si>
-    <t>what is the drug under study?</t>
-  </si>
-  <si>
-    <t>explain how drug works?</t>
-  </si>
-  <si>
-    <t>explain side effects and impacts w.r.to patient health?</t>
-  </si>
-  <si>
-    <t>what are the risks involved?</t>
-  </si>
-  <si>
-    <t>who is the sponsor for the study?</t>
-  </si>
-  <si>
-    <t>what is the medicalcare provided?</t>
-  </si>
-  <si>
-    <t>what is the trial period? (should be number of calendar days)</t>
-  </si>
-  <si>
-    <t>(optional) do you have any statistics for the number of participants participating?</t>
-  </si>
-  <si>
-    <t>Hello! We are conducting a clinical trial to investigate the effects of two different medications on the body's ability to absorb estrogens and progestogens. Participants will receive either cholestyramine or activated charcoal, and their plasma concentration will be measured after treatment. If your plasma concentration is above 0.02 μg/mL, you will receive feedback on this. It is important to note that both medications may reduce the effectiveness of oral contraceptives, so women who participate in the study will be recommended to use alternative contraceptive methods during the rapid elimination procedure. The Principal Investigator will review the contraindications of the rapid elimination medications before the procedure.
-If you experience a serious adverse event during the study, we may stop the study entirely. However, we do not offer compensation for research-related injuries. We encourage you to ask any questions you may have about the study and your participation before making a decision.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Sure! Here is the summary of the clinical trial procedures involved, highlighting important points that may be deciding factors for potential participants who may or may not want to join:
-As a participant in this study, you will undergo laboratory tests (CBC/CMP safety labs) to monitor your safety. If your lab results are more than twice the normal limits, you will be withdrawn from the study. Additionally, if three or more participants experience serious adverse events that are deemed related to participation in the study, the study will be stopped.</t>
-  </si>
-  <si>
-    <t>Sure! Here is the summary of the given text within two sentences: 
-If you are looking to participate in a clinical trial for colestipol hydrochloride and cholestyramine, be aware that you might experience gastrointestinal discomfort as a side effect. Additionally, certain medications should be taken at least an hour before or four hours after taking the study drug, and laboratory values will be monitored to ensure safe participation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Hello! We are looking for participants for our clinical trial to test the safety and efficacy of a new medication. The study will be stopped if 3 or more participants experience serious adverse events that are not deemed unrelated to participation in the study by the Principal Investigator or the independent safety monitoring physician. Additionally, if any participant's laboratory values (CBC/CMP safety labs) are greater than two times outside of the normal limits, they will be withdrawn from the study, and if three people are withdrawn for this reason, the study will be stopped. If you are interested in participating, please let us know!</t>
-  </si>
-  <si>
-    <t>Here is the summary of the clinical trial:
-Participants are needed for a clinical trial to evaluate the safety and effectiveness of two medications, colestipol hydrochloride and cholestyramine, in treating high cholesterol. The study will be stopped if three or more participants experience serious adverse events that are deemed related to the study. Participants will take the medications once a day for six weeks, and some may experience side effects such as nausea, vomiting, diarrhea, constipation, stomach pain, loss of appetite, or itching/irritation around the rectal area. It is important to note that colestipol hydrochloride should not be used if the participant has a blockage in their digestive tract and that concomitant medications should be taken at least one hour before or four hours after the study drug. If you are interested in participating, please contact us for more information.</t>
-  </si>
-  <si>
-    <t>Here are two possible summaries of the clinical trial procedures involved:
-1. Participants taking colestipol hydrochloride may experience gastrointestinal discomfort and should avoid concomitant medications, including oral contraceptives and over-the-counter vitamins, for at least one hour before or four hours after the study drug.
-2. Participants may experience side effects from cholestyramine or activated charcoal, such as nausea, stomach pain, loss of appetite, diarrhea, constipation, and itching/irritation around the rectal area. Women taking oral contraceptives should use alternative contraceptive methods during the rapid elimination procedure. The Principal Investigator will review the contraindications of the rapid elimination medications before the procedure.</t>
-  </si>
-  <si>
-    <t>Sure! Here is a summary of the procedures involved in the clinical trial: 
-If three or more participants experience serious adverse events deemed unrelated to participation in the study by the Principal Investigator or the independent safety monitoring physician, the whole study will be stopped. There will be no compensation for research-related injuries.</t>
-  </si>
-  <si>
-    <t>Here is a summary of the clinical trial in two sentences:
-Participants who receive teriflunomide treatment will undergo a rapid elimination procedure that may include cholestyramine or activated charcoal to measure plasma concentration, and those with high concentrations will receive feedback. The study may be stopped if serious adverse events occur in three or more participants, and alternative contraceptive methods are recommended for women during the procedure.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Hello! We are conducting a clinical trial for a new medication and we are looking for participants. Before deciding whether to participate, it is important to understand the potential risks and benefits of the study.
-Some safety endpoints to be aware of include: If any laboratory values (CBC/CMP safety labs) are more than two times outside of the normal limits, the participant will be withdrawn from the study. Additionally, if three or more participants experience serious adverse events that are deemed related to participation in the study, the study will be stopped. There will be no compensation for research-related injuries.
-The study will consist of 8 office visits and one phone call visit, and will last a total of 9 hours. Unscheduled visits or withdrawal visits may be necessary as needed. It is important to note that the study may be stopped early if serious adverse events occur.
-Please let us know if you have any questions or concerns before deciding whether to participate. We will be happy to provide more information and answer any questions you may have.</t>
-  </si>
-  <si>
-    <t>Hello there! We are currently recruiting participants for a clinical trial examining the safety and efficacy of a new medication. The study will involve 8 office visits over the course of several months, as well as one phone call visit. If you experience any serious adverse events during the study, we have a team of medical professionals who will be available to address any concerns you may have. Additionally, if you choose to withdraw from the study, we will work with you to schedule an unscheduled visit.
-Please note that the study may be stopped early if 3 or more participants experience serious adverse events that are deemed to be related to their participation in the study. This is done to ensure the safety of all participants. If you have any questions or concerns, please don't hesitate to reach out to us. We are here to support you throughout the study.</t>
+    <t>The participant may choose to join this clinical trial due to potential benefits and personal health improvements from receiving teriflunomide. This is particularly relevant given the significant elevations in liver enzymes (ALT, AST, or direct bilirubin) and/or ALT/AST ratio confirmed by retest. The risk of teratogenic effects associated with teriflunomide may also be a motivating factor for individuals who are pregnant or breast-feeding.
+The document does not explicitly mention potential benefits from the clinical trial, but rather outlines risks and safety protocols to ensure participant safety.</t>
+  </si>
+  <si>
+    <t>The primary objective of this clinical study is to evaluate teriflunomide, a new treatment method for liver-related issues such as elevated enzymes and impaired liver function.
+The study does not explicitly mention the type of outcomes being evaluated (e.g., efficacy, safety, or specific medical conditions). 
+The document does not explicitly mention this information.</t>
+  </si>
+  <si>
+    <t>The document does not explicitly mention the sponsor's name.
+The document does not explicitly confirm the study sponsor; however, it does provide information about potential risks to subjects, such as teratogenic effects and potential harm during pregnancy or breastfeeding. This suggests that the study is sponsored by a pharmaceutical company, but further confirmation would be necessary to determine the specific sponsor.</t>
+  </si>
+  <si>
+    <t>I'm happy to assist you with your query. However, I need more information about what specific aspect of the document you'd like me to focus on.
+Could you please clarify which detail from the document you'd like me to provide an answer for? Additionally, it would be helpful if you could specify whether you're looking for a general overview or a more detailed explanation of the mentioned aspect.</t>
+  </si>
+  <si>
+    <t>I can provide an answer to your question regarding the total duration of a clinical trial for an individual participant. 
+The document does not explicitly mention the specific duration of a clinical trial. It does, however, outline the requirements and restrictions for participating in the study, such as those related to pregnancy and liver function impairment.</t>
+  </si>
+  <si>
+    <t>You asked about potential side effects and risks listed in the document for participants. The document mentions several potential side effects and risks associated with teriflunomide, including:
+- Diarrhea
+- Nausea
+- Increased liver enzymes (AST and ALT)
+- Alopecia or hair loss/thinning
+- Influenza
+- Paresthesia
+It also states that participants should abstain from alcohol and drug use during the study due to potential interactions with teriflunomide. Additionally, prior use of investigational drugs in the preceding 6 months may raise concerns for liver function impairment or elevation.
+Regarding other conditions, the document mentions the following criteria under which participants would be excluded:
+- Pregnant or breastfeeding women
+- Women of childbearing potential not protected by effective contraception
+- Participants wishing to parent children during the course of the trial
+It also notes that participants with significantly impaired bone marrow function or anemia, leukopenia, or thrombocytopenia may be excluded from the study.</t>
+  </si>
+  <si>
+    <t>You are referring to Teriflunomide trials. The specific treatment being tested is Teriflunomide.
+The document does not explicitly mention a particular treatment or intervention for this trial, but it mentions that participants with significantly impaired bone marrow function or significant anemia (confirmed by retest) will require close monitoring of their hematocrit and white blood cell count during the study.</t>
+  </si>
+  <si>
+    <t>You're referring to question 8: What medical care is provided to participants during the trial? This question can be answered as follows:
+Routine procedures such as check-ups, lab tests, and monitoring are typically conducted by study staff throughout the duration of the trial. These include routine physical examinations, blood pressure checks, laboratory tests (e.g., CBC/CMP safety labs), and vital sign assessments. Additionally, participants may receive educational materials and information about their condition and treatment plan.
+The document does not explicitly mention specific medical care or treatments provided to participants during the trial.</t>
+  </si>
+  <si>
+    <t>I'm ready to assist you. However, I don't see a document provided. Please share the document with me, and I will analyze it and answer your questions in a formal, concise, and informative manner. If the document does not explicitly mention a specific detail, I will state that "The document does not explicitly mention this information."</t>
+  </si>
+  <si>
+    <t>You inquired about the ethical guidelines followed by this clinical trial. The document explicitly mentions informed consent and IRB approval as key components.
+The document does mention specific regulations, including those related to the use of investigational drugs such as teriflunomide, which is noted to be teratogenic and can cause harm to pregnant subjects or their partners.
+No information regarding recruitment methods, potential risks to subjects, or special population exclusion criteria is provided in the document.</t>
+  </si>
+  <si>
+    <t>The document does not explicitly mention specific statistical methods used for data analysis.
+However, the document mentions that blood samples will be collected via venipuncture and sent to Quest Diagnostics for processing. It also states that the results will be reported to the study team and may undergo genetic testing, which suggests that statistical analysis may be performed using techniques such as regression or logistic regression.</t>
+  </si>
+  <si>
+    <t>The document does not explicitly mention the final conclusions or recommendations based on the study. However, it provides a list of safety endpoints and risks associated with the teriflunomide treatment.
+The document does not explicitly mention any results that are pending due to participant withdrawal or loss of participants during the course of the trial.</t>
+  </si>
+  <si>
+    <t>The document does not explicitly mention the regulatory approvals or compliance measures specified in the document. However, it suggests that participants should comply with the standard regulations for clinical trials.
+To answer your query, the document does specify safety endpoints such as withdrawing a subject due to laboratory values exceeding normal limits (4.1) and risks associated with taking teriflunomide, including potential harm to subjects who become pregnant or their partners while taking the medication.</t>
+  </si>
+  <si>
+    <t>The document does not explicitly mention the specific phases of the trial. 
+The document mentions "Phases" but does not provide further clarification on what these phases entail.
+In clinical trials, participants typically undergo various stages or phases before receiving the investigational drug. The most common phases are:
+- Phase 1: Initial human studies to assess safety and tolerability.
+- Phase 2: Therapeutic efficacy evaluation in a smaller group of patients.
+- Phase 3: Large-scale, randomized controlled trials to confirm efficacy and monitor side effects.
+- Phase 4: Post-marketing surveillance and update on efficacy, safety, and any side effects associated with long-term use.
+These phases are not mentioned explicitly in the provided document.</t>
+  </si>
+  <si>
+    <t>You are seeking insights into the participant experience mentioned in the document, specifically regarding expectations, feedback, and participant rights.
+The document does mention participant rights, including the requirement for pregnant or breast-feeding women or those planning to become pregnant during the study to undergo a pregnancy test (13.3). It also mentions that participants wishing to parent children (be a partner in the conception of a child) during the course of the trial are not eligible.
+There is no mention of participant expectations within the document, but it does state that participants should abstain from alcohol and drug use due to potential risks associated with teriflunomide. However, it provides information on how such abstention can be facilitated through the study's recruitment methods (13.1-3).
+The document also includes a safety endpoint regarding laboratory values being greater than two times outside of normal limits, stating that the subject will be withdrawn if this occurs (15.1).</t>
   </si>
 </sst>
 </file>
@@ -451,7 +458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -466,83 +473,123 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>